<commit_message>
Algunas cositas en Cash
</commit_message>
<xml_diff>
--- a/Cash.xlsx
+++ b/Cash.xlsx
@@ -552,7 +552,7 @@
   <dimension ref="B2:N1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
+      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -573,11 +573,11 @@
       </c>
       <c r="C2" s="3" t="n">
         <f aca="false">H4*H5</f>
-        <v>100000</v>
+        <v>20000</v>
       </c>
       <c r="D2" s="4" t="n">
         <f aca="false">C2*$H$2</f>
-        <v>123500000</v>
+        <v>24700000</v>
       </c>
       <c r="E2" s="5" t="n">
         <f aca="false">D2/D2</f>
@@ -596,15 +596,15 @@
       </c>
       <c r="C3" s="3" t="n">
         <f aca="false">C8+C15+C18</f>
-        <v>51211.8796822105</v>
+        <v>10416.2253822105</v>
       </c>
       <c r="D3" s="9" t="n">
         <f aca="false">C3*$H$2</f>
-        <v>63246671.40753</v>
+        <v>12864038.34703</v>
       </c>
       <c r="E3" s="10" t="n">
         <f aca="false">D3/$D$2</f>
-        <v>0.512118796822105</v>
+        <v>0.520811269110526</v>
       </c>
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
@@ -616,21 +616,21 @@
       </c>
       <c r="C4" s="3" t="n">
         <f aca="false">C2-C8-C15-C18</f>
-        <v>48788.1203177895</v>
+        <v>9583.77461778948</v>
       </c>
       <c r="D4" s="13" t="n">
         <f aca="false">C4*$H$2</f>
-        <v>60253328.59247</v>
+        <v>11835961.65297</v>
       </c>
       <c r="E4" s="14" t="n">
         <f aca="false">D4/D2</f>
-        <v>0.487881203177895</v>
+        <v>0.479188730889474</v>
       </c>
       <c r="G4" s="15" t="s">
         <v>4</v>
       </c>
       <c r="H4" s="16" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -642,7 +642,7 @@
         <v>5</v>
       </c>
       <c r="H5" s="17" t="n">
-        <v>20000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -669,15 +669,15 @@
       </c>
       <c r="C8" s="19" t="n">
         <f aca="false">C9+C10+C11+C12+C13</f>
-        <v>8798.72825910931</v>
+        <v>2084.72825910931</v>
       </c>
       <c r="D8" s="20" t="n">
         <f aca="false">C8*$H$2</f>
-        <v>10866429.4</v>
+        <v>2574639.4</v>
       </c>
       <c r="E8" s="10" t="n">
         <f aca="false">D8/$D$2</f>
-        <v>0.0879872825910931</v>
+        <v>0.104236412955466</v>
       </c>
       <c r="G8" s="21"/>
       <c r="H8" s="21"/>
@@ -694,11 +694,11 @@
       </c>
       <c r="C9" s="23" t="n">
         <f aca="false">H4*H5*Porcentajes!C2</f>
-        <v>4400</v>
+        <v>880</v>
       </c>
       <c r="D9" s="20" t="n">
         <f aca="false">C9*$H$2</f>
-        <v>5434000</v>
+        <v>1086800</v>
       </c>
       <c r="G9" s="21"/>
       <c r="H9" s="21"/>
@@ -715,11 +715,11 @@
       </c>
       <c r="C10" s="23" t="n">
         <f aca="false">IF(H5&lt;H7,0,H4*H5*Porcentajes!C3)</f>
-        <v>4000</v>
+        <v>800</v>
       </c>
       <c r="D10" s="20" t="n">
         <f aca="false">C10*$H$2</f>
-        <v>4940000</v>
+        <v>988000</v>
       </c>
       <c r="G10" s="21"/>
       <c r="H10" s="21"/>
@@ -735,11 +735,12 @@
         <v>10</v>
       </c>
       <c r="C11" s="23" t="n">
-        <v>3.99</v>
+        <f aca="false">IF(H5&gt;500,9.99,3.99)</f>
+        <v>9.99</v>
       </c>
       <c r="D11" s="20" t="n">
         <f aca="false">C11*$H$2</f>
-        <v>4927.65</v>
+        <v>12337.65</v>
       </c>
       <c r="G11" s="21"/>
       <c r="H11" s="21"/>
@@ -812,16 +813,16 @@
         <v>13</v>
       </c>
       <c r="C15" s="19" t="n">
-        <f aca="false">IF(H5&lt;1500,0,C16)</f>
-        <v>16142.6250981377</v>
+        <f aca="false">IF((H4*H5)&lt;4000,0,C16)</f>
+        <v>3171.00309813765</v>
       </c>
       <c r="D15" s="20" t="n">
         <f aca="false">C15*$H$2</f>
-        <v>19936141.9962</v>
+        <v>3916188.8262</v>
       </c>
       <c r="E15" s="10" t="n">
         <f aca="false">D15/$D$2</f>
-        <v>0.161426250981377</v>
+        <v>0.158550154906883</v>
       </c>
       <c r="G15" s="21"/>
       <c r="H15" s="21"/>
@@ -838,11 +839,11 @@
       </c>
       <c r="C16" s="23" t="n">
         <f aca="false">(C2-C8)*Porcentajes!C4</f>
-        <v>16142.6250981377</v>
+        <v>3171.00309813765</v>
       </c>
       <c r="D16" s="20" t="n">
         <f aca="false">IF(C15=0,0,C16*$H$2)</f>
-        <v>19936141.9962</v>
+        <v>3916188.8262</v>
       </c>
       <c r="G16" s="21"/>
       <c r="H16" s="21"/>
@@ -868,16 +869,16 @@
         <v>15</v>
       </c>
       <c r="C18" s="19" t="n">
-        <f aca="false">IF(H5&lt;1500,0,C19)</f>
-        <v>26270.5263249636</v>
+        <f aca="false">IF((H4*H5)&lt;4000,0,C19)</f>
+        <v>5160.49402496356</v>
       </c>
       <c r="D18" s="20" t="n">
         <f aca="false">C18*$H$2</f>
-        <v>32444100.01133</v>
+        <v>6373210.12083</v>
       </c>
       <c r="E18" s="10" t="n">
         <f aca="false">D18/$D$2</f>
-        <v>0.262705263249636</v>
+        <v>0.258024701248178</v>
       </c>
       <c r="G18" s="21"/>
       <c r="H18" s="21"/>
@@ -894,11 +895,11 @@
       </c>
       <c r="C19" s="25" t="n">
         <f aca="false">(C2-C8-C15)*Porcentajes!C5</f>
-        <v>26270.5263249636</v>
+        <v>5160.49402496356</v>
       </c>
       <c r="D19" s="20" t="n">
         <f aca="false">IF(C18=0,0,C19*$H$2)</f>
-        <v>32444100.01133</v>
+        <v>6373210.12083</v>
       </c>
       <c r="E19" s="1"/>
       <c r="G19" s="21"/>

</xml_diff>